<commit_message>
Agregada demanda horaria en resultados p1
</commit_message>
<xml_diff>
--- a/resultados_p1.xlsx
+++ b/resultados_p1.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10513"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc\Desktop\Cosas\Universidad\11° Semestre\Operación Económica\Operacion-Economica\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felipenoris/tmp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F679D51-0E68-4137-A804-F04D27B6D88D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C353BCB8-5EC8-0143-BDD3-A1B661DAACD7}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{52D9C27D-0EF6-DD41-9728-0267E68F7539}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{52D9C27D-0EF6-DD41-9728-0267E68F7539}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Estado ON-OFF" sheetId="2" r:id="rId2"/>
-    <sheet name="Generación" sheetId="3" r:id="rId3"/>
-    <sheet name="Costos" sheetId="4" r:id="rId4"/>
+    <sheet name="Estado ON-OFF" r:id="rId4" sheetId="2"/>
+    <sheet name="Generación" r:id="rId5" sheetId="3"/>
+    <sheet name="Costos" r:id="rId7" sheetId="4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="15">
   <si>
     <t>Hora</t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t>Generador 7</t>
+  </si>
+  <si>
+    <t>Demanda horaria</t>
   </si>
   <si>
     <t>Variable</t>
@@ -125,9 +128,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -165,7 +168,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -271,7 +274,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -413,33 +416,33 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C2E5552-FF33-4CBF-919C-762896CC90FA}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
+  <dimension ref="A1:A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97EEB053-D658-4396-BCB8-888B48666819}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -465,628 +468,628 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="G2">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="H2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="H3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>-0.0</v>
       </c>
       <c r="G4">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="H4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>-0.0</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>-0.0</v>
       </c>
       <c r="G5">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="H5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>-0.0</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>-0.0</v>
       </c>
       <c r="G6">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="H6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>-0.0</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>-0.0</v>
       </c>
       <c r="G7">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="H7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>-0.0</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>-0.0</v>
       </c>
       <c r="G8">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="H8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>-0.0</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>-0.0</v>
       </c>
       <c r="G9">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="H9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>-0.0</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>-0.0</v>
       </c>
       <c r="G10">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="H10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>-0.0</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>-0.0</v>
       </c>
       <c r="G11">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="H11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="C12">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>-0.0</v>
       </c>
       <c r="G12">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="H12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="D13">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="F13">
-        <v>0</v>
+        <v>-0.0</v>
       </c>
       <c r="G13">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="H13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="D14">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="E14">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="F14">
-        <v>0</v>
+        <v>-0.0</v>
       </c>
       <c r="G14">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="H14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="D15">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="E15">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="F15">
-        <v>0</v>
+        <v>-0.0</v>
       </c>
       <c r="G15">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="H15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="C16">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="D16">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="E16">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="F16">
-        <v>0</v>
+        <v>-0.0</v>
       </c>
       <c r="G16">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="H16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="C17">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="D17">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="E17">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="F17">
-        <v>0</v>
+        <v>-0.0</v>
       </c>
       <c r="G17">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="H17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="C18">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="D18">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="E18">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="F18">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="G18">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="H18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="C19">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="D19">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="E19">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="F19">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="G19">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="H19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="C20">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="D20">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="E20">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="F20">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="G20">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="H20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="C21">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="D21">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="E21">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="F21">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="G21">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="H21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="C22">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="D22">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="E22">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="F22">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="G22">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="H22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="C23">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="D23">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="E23">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="F23">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="G23">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="H23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="C24">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="D24">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="E24">
-        <v>0</v>
+        <v>-0.0</v>
       </c>
       <c r="F24">
-        <v>0</v>
+        <v>-0.0</v>
       </c>
       <c r="G24">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="H24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="C25">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="D25">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="E25">
-        <v>0</v>
+        <v>-0.0</v>
       </c>
       <c r="F25">
-        <v>0</v>
+        <v>-0.0</v>
       </c>
       <c r="G25">
-        <v>1</v>
+        <v>1.0</v>
       </c>
       <c r="H25">
-        <v>1</v>
+        <v>1.0</v>
       </c>
     </row>
   </sheetData>
@@ -1095,14 +1098,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{650E04E9-24C9-45C9-A608-EBCFEABD3B6F}">
-  <dimension ref="A1:H25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
+  <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1127,117 +1130,132 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>100</v>
+        <v>100.0</v>
       </c>
       <c r="C2">
-        <v>74.999999999999943</v>
+        <v>74.99999999999994</v>
       </c>
       <c r="D2">
         <v>52.83297191515399</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="G2">
         <v>31.167028084846212</v>
       </c>
       <c r="H2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+        <v>0.0</v>
+      </c>
+      <c r="I2">
+        <v>258.99999999999994</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>98.941418522032436</v>
+        <v>98.94141852203244</v>
       </c>
       <c r="C3">
         <v>52.499999999999986</v>
       </c>
       <c r="D3">
-        <v>30.332971915154339</v>
+        <v>30.33297191515434</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="G3">
         <v>29.425609562813513</v>
       </c>
       <c r="H3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+        <v>0.0</v>
+      </c>
+      <c r="I3">
+        <v>211.20000000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>100</v>
+        <v>100.0</v>
       </c>
       <c r="C4">
-        <v>50.094737398499838</v>
+        <v>50.09473739849984</v>
       </c>
       <c r="D4">
-        <v>7.8329719151546939</v>
+        <v>7.832971915154694</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="G4">
         <v>27.672290686345676</v>
       </c>
       <c r="H4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+        <v>0.0</v>
+      </c>
+      <c r="I4">
+        <v>185.60000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
-        <v>100</v>
+        <v>100.0</v>
       </c>
       <c r="C5">
-        <v>30.267747395165252</v>
+        <v>30.26774739516525</v>
       </c>
       <c r="D5">
         <v>7.4999999999998765</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="G5">
         <v>28.632252604835134</v>
       </c>
       <c r="H5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+        <v>0.0</v>
+      </c>
+      <c r="I5">
+        <v>166.40000000000003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
-        <v>98.117104776268107</v>
+        <v>98.1171047762681</v>
       </c>
       <c r="C6">
         <v>25.631490982206827</v>
@@ -1246,24 +1264,27 @@
         <v>7.5</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="G6">
         <v>28.751256148226485</v>
       </c>
       <c r="H6">
-        <v>1.4809329877823026E-4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+        <v>0.00014809329877823026</v>
+      </c>
+      <c r="I6">
+        <v>160.00000000000003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7">
-        <v>100</v>
+        <v>100.0</v>
       </c>
       <c r="C7">
         <v>48.13149098220677</v>
@@ -1272,24 +1293,27 @@
         <v>7.5</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="G7">
         <v>29.223303538341348</v>
       </c>
       <c r="H7">
-        <v>7.1452054794520539</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+        <v>7.145205479452054</v>
+      </c>
+      <c r="I7">
+        <v>192.00000000000003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8">
-        <v>100</v>
+        <v>100.0</v>
       </c>
       <c r="C8">
         <v>55.748045697290195</v>
@@ -1298,10 +1322,10 @@
         <v>7.5</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="G8">
         <v>28.636219389714864</v>
@@ -1309,51 +1333,57 @@
       <c r="H8">
         <v>32.11573491299513</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I8">
+        <v>224.00000000000003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9">
-        <v>100</v>
+        <v>100.0</v>
       </c>
       <c r="C9">
-        <v>74.999999999999915</v>
+        <v>74.99999999999991</v>
       </c>
       <c r="D9">
-        <v>8.7692181907237146</v>
+        <v>8.769218190723715</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="G9">
-        <v>29.738985560973511</v>
+        <v>29.73898556097351</v>
       </c>
       <c r="H9">
         <v>36.091796248303055</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I9">
+        <v>249.60000000000008</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10">
-        <v>100</v>
+        <v>100.0</v>
       </c>
       <c r="C10">
-        <v>74.999999999999943</v>
+        <v>74.99999999999994</v>
       </c>
       <c r="D10">
-        <v>20.886931207143391</v>
+        <v>20.88693120714339</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="G10">
         <v>30.42127254455378</v>
@@ -1361,77 +1391,86 @@
       <c r="H10">
         <v>36.091796248303055</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I10">
+        <v>262.40000000000003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11">
-        <v>100</v>
+        <v>100.0</v>
       </c>
       <c r="C11">
-        <v>74.999999999999943</v>
+        <v>74.99999999999994</v>
       </c>
       <c r="D11">
-        <v>38.742191163703978</v>
+        <v>38.74219116370398</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="G11">
-        <v>31.766012587993242</v>
+        <v>31.76601258799324</v>
       </c>
       <c r="H11">
         <v>36.091796248303055</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I11">
+        <v>281.6000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12">
-        <v>100</v>
+        <v>100.0</v>
       </c>
       <c r="C12">
-        <v>74.999999999999972</v>
+        <v>74.99999999999997</v>
       </c>
       <c r="D12">
         <v>40.577617196299315</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="G12">
-        <v>33.130586555397841</v>
+        <v>33.13058655539784</v>
       </c>
       <c r="H12">
         <v>36.091796248303055</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I12">
+        <v>284.80000000000007</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13">
-        <v>100</v>
+        <v>100.0</v>
       </c>
       <c r="C13">
-        <v>74.999999999999957</v>
+        <v>74.99999999999996</v>
       </c>
       <c r="D13">
         <v>23.400804375724494</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="F13">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="G13">
         <v>34.3073993759728</v>
@@ -1439,25 +1478,28 @@
       <c r="H13">
         <v>36.091796248303055</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I13">
+        <v>268.80000000000007</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14">
-        <v>100</v>
+        <v>100.0</v>
       </c>
       <c r="C14">
-        <v>74.999999999999943</v>
+        <v>74.99999999999994</v>
       </c>
       <c r="D14">
         <v>10.600804375724474</v>
       </c>
       <c r="E14">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="F14">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="G14">
         <v>34.3073993759728</v>
@@ -1465,25 +1507,28 @@
       <c r="H14">
         <v>36.091796248303055</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I14">
+        <v>256.00000000000006</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15">
-        <v>100</v>
+        <v>100.0</v>
       </c>
       <c r="C15">
-        <v>59.099999999999831</v>
+        <v>59.09999999999983</v>
       </c>
       <c r="D15">
         <v>13.700804375724449</v>
       </c>
       <c r="E15">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="F15">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="G15">
         <v>34.3073993759728</v>
@@ -1491,25 +1536,28 @@
       <c r="H15">
         <v>36.091796248303055</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I15">
+        <v>243.20000000000005</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16">
-        <v>100</v>
+        <v>100.0</v>
       </c>
       <c r="C16">
-        <v>74.999999999999972</v>
+        <v>74.99999999999997</v>
       </c>
       <c r="D16">
-        <v>36.200804375724253</v>
+        <v>36.20080437572425</v>
       </c>
       <c r="E16">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="F16">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="G16">
         <v>34.3073993759728</v>
@@ -1517,25 +1565,28 @@
       <c r="H16">
         <v>36.091796248303055</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I16">
+        <v>281.6000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17">
-        <v>100</v>
+        <v>100.0</v>
       </c>
       <c r="C17">
-        <v>74.999999999999957</v>
+        <v>74.99999999999996</v>
       </c>
       <c r="D17">
-        <v>42.600804375724287</v>
+        <v>42.60080437572429</v>
       </c>
       <c r="E17">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="F17">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="G17">
         <v>34.3073993759728</v>
@@ -1543,25 +1594,28 @@
       <c r="H17">
         <v>36.091796248303055</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I17">
+        <v>288.0000000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18">
-        <v>100</v>
+        <v>100.0</v>
       </c>
       <c r="C18">
-        <v>63.341043440700851</v>
+        <v>63.34104344070085</v>
       </c>
       <c r="D18">
-        <v>38.259760935023579</v>
+        <v>38.25976093502358</v>
       </c>
       <c r="E18">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="F18">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="G18">
         <v>34.3073993759728</v>
@@ -1569,25 +1623,28 @@
       <c r="H18">
         <v>36.091796248303055</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I18">
+        <v>272.00000000000006</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19">
-        <v>100</v>
+        <v>100.0</v>
       </c>
       <c r="C19">
-        <v>74.999999999999915</v>
+        <v>74.99999999999991</v>
       </c>
       <c r="D19">
-        <v>60.759760935023401</v>
+        <v>60.7597609350234</v>
       </c>
       <c r="E19">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="F19">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="G19">
         <v>34.3073993759728</v>
@@ -1595,161 +1652,182 @@
       <c r="H19">
         <v>14.732839689004052</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I19">
+        <v>284.80000000000007</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20">
-        <v>100</v>
+        <v>100.0</v>
       </c>
       <c r="C20">
-        <v>74.999999999999915</v>
+        <v>74.99999999999991</v>
       </c>
       <c r="D20">
-        <v>74.999999999999972</v>
+        <v>74.99999999999997</v>
       </c>
       <c r="E20">
         <v>15.870460675860121</v>
       </c>
       <c r="F20">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="G20">
         <v>34.3073993759728</v>
       </c>
       <c r="H20">
-        <v>0.62213994816734319</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+        <v>0.6221399481673432</v>
+      </c>
+      <c r="I20">
+        <v>300.8000000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21">
-        <v>100</v>
+        <v>100.0</v>
       </c>
       <c r="C21">
-        <v>74.999999999999943</v>
+        <v>74.99999999999994</v>
       </c>
       <c r="D21">
-        <v>75</v>
+        <v>75.0</v>
       </c>
       <c r="E21">
         <v>29.292600624027642</v>
       </c>
       <c r="F21">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="G21">
         <v>34.3073993759728</v>
       </c>
       <c r="H21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+        <v>0.0</v>
+      </c>
+      <c r="I21">
+        <v>313.6000000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22">
-        <v>100</v>
+        <v>100.0</v>
       </c>
       <c r="C22">
-        <v>74.999999999999972</v>
+        <v>74.99999999999997</v>
       </c>
       <c r="D22">
-        <v>75</v>
+        <v>75.0</v>
       </c>
       <c r="E22">
         <v>35.692600624026774</v>
       </c>
       <c r="F22">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="G22">
         <v>34.3073993759728</v>
       </c>
       <c r="H22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+        <v>0.0</v>
+      </c>
+      <c r="I22">
+        <v>320.00000000000006</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23">
-        <v>100</v>
+        <v>100.0</v>
       </c>
       <c r="C23">
-        <v>74.999999999999957</v>
+        <v>74.99999999999996</v>
       </c>
       <c r="D23">
-        <v>65.499999999999446</v>
+        <v>65.49999999999945</v>
       </c>
       <c r="E23">
         <v>13.192600624027444</v>
       </c>
       <c r="F23">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="G23">
         <v>34.3073993759728</v>
       </c>
       <c r="H23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+        <v>0.0</v>
+      </c>
+      <c r="I23">
+        <v>288.0000000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24">
-        <v>100</v>
+        <v>100.0</v>
       </c>
       <c r="C24">
-        <v>74.999999999999929</v>
+        <v>74.99999999999993</v>
       </c>
       <c r="D24">
-        <v>70.896165441548121</v>
+        <v>70.89616544154812</v>
       </c>
       <c r="E24">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="F24">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="G24">
-        <v>32.503834558452162</v>
+        <v>32.50383455845216</v>
       </c>
       <c r="H24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+        <v>0.0</v>
+      </c>
+      <c r="I24">
+        <v>278.40000000000003</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25">
-        <v>100</v>
+        <v>100.0</v>
       </c>
       <c r="C25">
-        <v>74.999999999999986</v>
+        <v>74.99999999999999</v>
       </c>
       <c r="D25">
         <v>56.193304067182915</v>
       </c>
       <c r="E25">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="F25">
-        <v>0</v>
+        <v>0.0</v>
       </c>
       <c r="G25">
         <v>31.206695932817297</v>
       </c>
       <c r="H25">
-        <v>0</v>
+        <v>0.0</v>
+      </c>
+      <c r="I25">
+        <v>262.40000000000003</v>
       </c>
     </row>
   </sheetData>
@@ -1758,56 +1836,51 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C24CE8F-2BF4-4FF0-B79A-1A16F7AD30F2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
+    <sheetView tabSelected="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="22.59765625" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B2">
         <v>218792.88691128805</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B3">
-        <v>9750</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+        <v>9750.0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B4">
-        <v>37800</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+        <v>37800.0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B5">
-        <v>171242.88691128811</v>
+        <v>171242.8869112881</v>
       </c>
     </row>
   </sheetData>

</xml_diff>